<commit_message>
format parsing similar to micropos
</commit_message>
<xml_diff>
--- a/log ciptascope.xlsx
+++ b/log ciptascope.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7680" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>R15</t>
   </si>
@@ -66,6 +67,63 @@
   </si>
   <si>
     <t>z</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Device</t>
+  </si>
+  <si>
+    <t>baudarate</t>
+  </si>
+  <si>
+    <t>freq</t>
+  </si>
+  <si>
+    <t>reader</t>
+  </si>
+  <si>
+    <t>samsung a3</t>
+  </si>
+  <si>
+    <t>nokia lama</t>
+  </si>
+  <si>
+    <t>iphone 5se</t>
+  </si>
+  <si>
+    <t>iphone 6plus</t>
+  </si>
+  <si>
+    <t>iphone 4</t>
+  </si>
+  <si>
+    <t>freq tidak dapat</t>
+  </si>
+  <si>
+    <t>oppo</t>
+  </si>
+  <si>
+    <t>huawei p8</t>
+  </si>
+  <si>
+    <t>redmi</t>
+  </si>
+  <si>
+    <t>hang setelah command 00 88</t>
+  </si>
+  <si>
+    <t>xpria z2</t>
+  </si>
+  <si>
+    <t>ace z500</t>
+  </si>
+  <si>
+    <t>iphone 4 se</t>
+  </si>
+  <si>
+    <t>menunggu perbaikan chip emulator</t>
   </si>
 </sst>
 </file>
@@ -429,7 +487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
@@ -719,4 +777,208 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B5:G17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="26.140625" customWidth="1"/>
+    <col min="4" max="4" width="33.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6">
+        <v>9600</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7">
+        <v>10000</v>
+      </c>
+      <c r="E7">
+        <v>3850000</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>8800</v>
+      </c>
+      <c r="E8">
+        <v>3200000</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9">
+        <v>12800</v>
+      </c>
+      <c r="E9">
+        <v>4700000</v>
+      </c>
+      <c r="F9">
+        <v>10000</v>
+      </c>
+      <c r="G9">
+        <v>38500000</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10">
+        <v>12800</v>
+      </c>
+      <c r="E10">
+        <v>4700000</v>
+      </c>
+      <c r="F10">
+        <v>10000</v>
+      </c>
+      <c r="G10">
+        <v>38500000</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12">
+        <v>10000</v>
+      </c>
+      <c r="E12">
+        <v>3850000</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13">
+        <v>10000</v>
+      </c>
+      <c r="E13">
+        <v>3850000</v>
+      </c>
+      <c r="F13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14">
+        <v>10000</v>
+      </c>
+      <c r="E14">
+        <v>3850000</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15">
+        <v>10000</v>
+      </c>
+      <c r="E15">
+        <v>3850000</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>